<commit_message>
Added shell casing and footsteps sounds
</commit_message>
<xml_diff>
--- a/Assets/Sound/Licenses.xlsx
+++ b/Assets/Sound/Licenses.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1002D7-7FEA-49A1-AAE3-5818913ABBCA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A1AFCD-0DAF-4F7E-AF8C-23DEBF31E392}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Sound Name</t>
   </si>
@@ -59,6 +59,24 @@
   </si>
   <si>
     <t>http://soundbible.com/1927-50-Cal-CasingX3.html</t>
+  </si>
+  <si>
+    <t>Artist</t>
+  </si>
+  <si>
+    <t>Publication Date</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Ghost Rider</t>
+  </si>
+  <si>
+    <t>Tim Fryer</t>
+  </si>
+  <si>
+    <t>http://soundbible.com/2057-Footsteps-On-Cement.html</t>
   </si>
 </sst>
 </file>
@@ -103,9 +121,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -387,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -400,9 +419,11 @@
     <col min="3" max="3" width="25.1796875" customWidth="1"/>
     <col min="4" max="4" width="19.36328125" customWidth="1"/>
     <col min="5" max="5" width="31.7265625" customWidth="1"/>
+    <col min="6" max="6" width="18.08984375" customWidth="1"/>
+    <col min="7" max="7" width="53.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -416,10 +437,16 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -432,11 +459,14 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -450,12 +480,34 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2">
+        <v>40005</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2">
+        <v>41346</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{59938AB5-9116-43E6-90AE-D84C432FCA3C}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{59938AB5-9116-43E6-90AE-D84C432FCA3C}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{EFC4A4C7-67B0-47F0-A408-50D141A765E4}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{9CABD4C9-141A-4936-B5E9-484FCB9722F1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>